<commit_message>
Deploying to gh-pages from  @ 23244c7570684dfd18bbcd1d4c3077ca9f03ed12 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-3-1.xlsx
+++ b/assets/excel/2021_1-3-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEF2A84-E3F2-4FB0-9FF6-DEA93BD8122D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F31398-753D-4444-84A2-13B20BB78CFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{CD3F59CD-FBB8-4114-883D-A6BBE5CD1D50}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="78">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
+  <si>
+    <t>4) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes</t>
   </si>
 </sst>
 </file>
@@ -641,6 +644,9 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -676,9 +682,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -996,9 +999,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DBC63E-FF2A-48D5-9066-9477AC3D1A19}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:J488"/>
+  <dimension ref="B1:J489"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
@@ -1035,10 +1038,10 @@
       <c r="F4" s="8"/>
     </row>
     <row r="7" spans="2:10" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="46" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="9" t="s">
@@ -1061,18 +1064,18 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="44"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47">
+      <c r="C8" s="45"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48">
         <v>1000</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="50" t="s">
+      <c r="F8" s="49"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
     </row>
     <row r="9" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="12">
@@ -14676,86 +14679,98 @@
       <c r="C478" s="27"/>
     </row>
     <row r="479" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C479" s="52" t="s">
+      <c r="C479" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="D479" s="52"/>
-      <c r="E479" s="52"/>
-      <c r="F479" s="52"/>
-      <c r="G479" s="52"/>
-      <c r="H479" s="52"/>
-      <c r="I479" s="52"/>
-      <c r="J479" s="52"/>
+      <c r="D479" s="53"/>
+      <c r="E479" s="53"/>
+      <c r="F479" s="53"/>
+      <c r="G479" s="53"/>
+      <c r="H479" s="53"/>
+      <c r="I479" s="53"/>
+      <c r="J479" s="53"/>
     </row>
     <row r="480" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C480" s="53" t="s">
+      <c r="C480" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D480" s="53"/>
-      <c r="E480" s="53"/>
-      <c r="F480" s="53"/>
-      <c r="G480" s="53"/>
-      <c r="H480" s="53"/>
-      <c r="I480" s="53"/>
-      <c r="J480" s="53"/>
+      <c r="D480" s="54"/>
+      <c r="E480" s="54"/>
+      <c r="F480" s="54"/>
+      <c r="G480" s="54"/>
+      <c r="H480" s="54"/>
+      <c r="I480" s="54"/>
+      <c r="J480" s="54"/>
     </row>
     <row r="481" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C481" s="42" t="s">
+      <c r="C481" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="D481" s="42"/>
-      <c r="E481" s="42"/>
-      <c r="F481" s="42"/>
-      <c r="G481" s="42"/>
-      <c r="H481" s="42"/>
-      <c r="I481" s="42"/>
-      <c r="J481" s="42"/>
-    </row>
-    <row r="482" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C482" s="28"/>
-      <c r="D482" s="28"/>
-      <c r="E482" s="28"/>
-      <c r="F482" s="28"/>
-      <c r="G482" s="28"/>
-      <c r="H482" s="28"/>
-      <c r="I482" s="28"/>
-      <c r="J482" s="28"/>
+      <c r="D481" s="43"/>
+      <c r="E481" s="43"/>
+      <c r="F481" s="43"/>
+      <c r="G481" s="43"/>
+      <c r="H481" s="43"/>
+      <c r="I481" s="43"/>
+      <c r="J481" s="43"/>
+    </row>
+    <row r="482" spans="3:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C482" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D482" s="43"/>
+      <c r="E482" s="43"/>
+      <c r="F482" s="43"/>
+      <c r="G482" s="43"/>
+      <c r="H482" s="43"/>
+      <c r="I482" s="43"/>
+      <c r="J482" s="43"/>
     </row>
     <row r="483" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C483" s="29" t="s">
+      <c r="C483" s="28"/>
+      <c r="D483" s="28"/>
+      <c r="E483" s="28"/>
+      <c r="F483" s="28"/>
+      <c r="G483" s="28"/>
+      <c r="H483" s="28"/>
+      <c r="I483" s="28"/>
+      <c r="J483" s="28"/>
+    </row>
+    <row r="484" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C484" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="D483" s="30"/>
-      <c r="E483" s="31"/>
-      <c r="F483" s="31"/>
-      <c r="G483" s="31"/>
-      <c r="H483" s="32"/>
-      <c r="I483" s="32"/>
-      <c r="J483"/>
-    </row>
-    <row r="484" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C485" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
+      <c r="D484" s="30"/>
+      <c r="E484" s="31"/>
+      <c r="F484" s="31"/>
+      <c r="G484" s="31"/>
+      <c r="H484" s="32"/>
+      <c r="I484" s="32"/>
+      <c r="J484"/>
+    </row>
+    <row r="485" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="486" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C486" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="487" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C487" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="488" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C488" s="29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="488" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C488" s="54" t="s">
+    <row r="489" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C489" s="42" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="C481:J481"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
@@ -14763,9 +14778,10 @@
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="C479:J479"/>
     <mergeCell ref="C480:J480"/>
+    <mergeCell ref="C482:J482"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C488" r:id="rId1" xr:uid="{28589D7B-1300-4EC0-9CD3-76B748533734}"/>
+    <hyperlink ref="C489" r:id="rId1" xr:uid="{28589D7B-1300-4EC0-9CD3-76B748533734}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>